<commit_message>
updated the business requirements folder
</commit_message>
<xml_diff>
--- a/business_requirements/Agents/Supplier Ranking/Formulas and Ranking/Pricing Matrix_Ranking_Policy Engine.xlsx
+++ b/business_requirements/Agents/Supplier Ranking/Formulas and Ranking/Pricing Matrix_Ranking_Policy Engine.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29212"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://beyondprocwise.sharepoint.com/sites/development/Shared Documents/Agents/Supplier Ranking/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A295A813-A348-45CD-810C-D44B16992A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{A295A813-A348-45CD-810C-D44B16992A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB0658CD-FAA7-4B11-92B5-3165E1B2D975}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -34,6 +50,9 @@
     <t>Example Value</t>
   </si>
   <si>
+    <t xml:space="preserve">Unit </t>
+  </si>
+  <si>
     <t>Weighting</t>
   </si>
   <si>
@@ -64,466 +83,469 @@
     <t>Acceptance</t>
   </si>
   <si>
+    <t>Acceptance Time</t>
+  </si>
+  <si>
+    <t>24 hours</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Policy Agent</t>
+  </si>
+  <si>
+    <t>3 days</t>
+  </si>
+  <si>
+    <t>7 days</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Field Service</t>
+  </si>
+  <si>
+    <t>Remote Support</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
     <t>Company Structure / Commitment</t>
   </si>
   <si>
+    <t>Committed Contract Term</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3 years</t>
+  </si>
+  <si>
+    <t>3-5 years</t>
+  </si>
+  <si>
+    <t>5-7 years</t>
+  </si>
+  <si>
+    <t>7+ years</t>
+  </si>
+  <si>
+    <t>Corporate Guarantees</t>
+  </si>
+  <si>
+    <t>Parent Co</t>
+  </si>
+  <si>
+    <t>Bank Guarantee</t>
+  </si>
+  <si>
+    <t>Country of Registration</t>
+  </si>
+  <si>
+    <t>UK</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Joint Venture</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Listed Status</t>
+  </si>
+  <si>
+    <t>Public</t>
+  </si>
+  <si>
+    <t>Private</t>
+  </si>
+  <si>
+    <t>SME/Local Ownership</t>
+  </si>
+  <si>
     <t>Date &amp; Product History</t>
   </si>
   <si>
+    <t>Product Age</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>1-2 years</t>
+  </si>
+  <si>
+    <t>&gt;2 years</t>
+  </si>
+  <si>
+    <t>Technology Refresh Cycle</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>Bi-Annual</t>
+  </si>
+  <si>
+    <t>5-year</t>
+  </si>
+  <si>
+    <t>Ad hoc</t>
+  </si>
+  <si>
     <t>Delivery Terms</t>
   </si>
   <si>
+    <t>Last-Mile Logistics</t>
+  </si>
+  <si>
+    <t>Included</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Excluded</t>
+  </si>
+  <si>
+    <t>Lead Time</t>
+  </si>
+  <si>
+    <t>1 week</t>
+  </si>
+  <si>
+    <t>2 weeks</t>
+  </si>
+  <si>
+    <t>4+ weeks</t>
+  </si>
+  <si>
+    <t>On-Time Delivery Guarantee</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
+    <t>98%</t>
+  </si>
+  <si>
+    <t>99.50%</t>
+  </si>
+  <si>
+    <t>Partial Shipments</t>
+  </si>
+  <si>
+    <t>Allowed</t>
+  </si>
+  <si>
+    <t>Not Allowed</t>
+  </si>
+  <si>
     <t>Discount Structures</t>
   </si>
   <si>
+    <t>Early Payment Discount</t>
+  </si>
+  <si>
+    <t>1%</t>
+  </si>
+  <si>
+    <t>Supplier Ranking Agent</t>
+  </si>
+  <si>
+    <t>2%</t>
+  </si>
+  <si>
+    <t>3%</t>
+  </si>
+  <si>
+    <t>Total Contract Value Discount</t>
+  </si>
+  <si>
+    <t>5%</t>
+  </si>
+  <si>
+    <t>10%</t>
+  </si>
+  <si>
+    <t>15%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>Volume-Based Incentives</t>
+  </si>
+  <si>
+    <t>Tiered</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
     <t>Geography Scope</t>
   </si>
   <si>
+    <t>Coverage</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Support Regions</t>
+  </si>
+  <si>
+    <t>Local Only</t>
+  </si>
+  <si>
+    <t>EU + UK</t>
+  </si>
+  <si>
     <t>Insurance &amp; Liability</t>
   </si>
   <si>
+    <t>Cyber Insurance</t>
+  </si>
+  <si>
+    <t>£500k</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>£1M</t>
+  </si>
+  <si>
+    <t>General Liability Insurance</t>
+  </si>
+  <si>
+    <t>£5M</t>
+  </si>
+  <si>
+    <t>£10M</t>
+  </si>
+  <si>
+    <t>Indemnity Cap</t>
+  </si>
+  <si>
+    <t>1x contract</t>
+  </si>
+  <si>
+    <t>2x contract</t>
+  </si>
+  <si>
+    <t>Unlimited</t>
+  </si>
+  <si>
     <t>Payment Release Triggers</t>
   </si>
   <si>
+    <t>Deliverable Approval</t>
+  </si>
+  <si>
+    <t>Internal QA</t>
+  </si>
+  <si>
+    <t>3rd Party Certifier</t>
+  </si>
+  <si>
+    <t>Not Required</t>
+  </si>
+  <si>
+    <t>Milestone-Based Payments</t>
+  </si>
+  <si>
     <t>Payment Terms</t>
   </si>
   <si>
+    <t>Days to Payment</t>
+  </si>
+  <si>
+    <t>30 days</t>
+  </si>
+  <si>
+    <t>60 days</t>
+  </si>
+  <si>
+    <t>90 days</t>
+  </si>
+  <si>
+    <t>Early Payment Discounts</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
     <t>Regulatory Compliance</t>
   </si>
   <si>
+    <t>GDPR Compliance</t>
+  </si>
+  <si>
+    <t>ISO 27001 Certification</t>
+  </si>
+  <si>
+    <t>Modern Slavery Statement</t>
+  </si>
+  <si>
     <t>Service Levels</t>
   </si>
   <si>
+    <t>Resolution Time</t>
+  </si>
+  <si>
+    <t>24 hrs</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>48 hrs</t>
+  </si>
+  <si>
+    <t>72 hrs</t>
+  </si>
+  <si>
+    <t>Response Time</t>
+  </si>
+  <si>
+    <t>4 hrs</t>
+  </si>
+  <si>
+    <t>8 hrs</t>
+  </si>
+  <si>
+    <t>Next Day</t>
+  </si>
+  <si>
+    <t>Service Credits</t>
+  </si>
+  <si>
     <t>Warranty &amp; Support</t>
   </si>
   <si>
+    <t>Spare Parts Availability</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Support SLA</t>
+  </si>
+  <si>
+    <t>8x5</t>
+  </si>
+  <si>
+    <t>24x5</t>
+  </si>
+  <si>
+    <t>24x7</t>
+  </si>
+  <si>
+    <t>Warranty Duration</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
     <t>Pricing</t>
   </si>
   <si>
-    <t>Acceptance Time</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Committed Contract Term</t>
-  </si>
-  <si>
-    <t>Corporate Guarantees</t>
-  </si>
-  <si>
-    <t>Country of Registration</t>
-  </si>
-  <si>
-    <t>Joint Venture</t>
-  </si>
-  <si>
-    <t>Listed Status</t>
-  </si>
-  <si>
-    <t>SME/Local Ownership</t>
-  </si>
-  <si>
-    <t>Product Age</t>
-  </si>
-  <si>
-    <t>Technology Refresh Cycle</t>
-  </si>
-  <si>
-    <t>Last-Mile Logistics</t>
-  </si>
-  <si>
-    <t>Lead Time</t>
-  </si>
-  <si>
-    <t>On-Time Delivery Guarantee</t>
-  </si>
-  <si>
-    <t>Partial Shipments</t>
-  </si>
-  <si>
-    <t>Early Payment Discount</t>
-  </si>
-  <si>
-    <t>Total Contract Value Discount</t>
-  </si>
-  <si>
-    <t>Volume-Based Incentives</t>
-  </si>
-  <si>
-    <t>Coverage</t>
-  </si>
-  <si>
-    <t>Support Regions</t>
-  </si>
-  <si>
-    <t>Cyber Insurance</t>
-  </si>
-  <si>
-    <t>General Liability Insurance</t>
-  </si>
-  <si>
-    <t>Indemnity Cap</t>
-  </si>
-  <si>
-    <t>Deliverable Approval</t>
-  </si>
-  <si>
-    <t>Milestone-Based Payments</t>
-  </si>
-  <si>
-    <t>Days to Payment</t>
-  </si>
-  <si>
-    <t>Early Payment Discounts</t>
-  </si>
-  <si>
-    <t>GDPR Compliance</t>
-  </si>
-  <si>
-    <t>ISO 27001 Certification</t>
-  </si>
-  <si>
-    <t>Modern Slavery Statement</t>
-  </si>
-  <si>
-    <t>Resolution Time</t>
-  </si>
-  <si>
-    <t>Response Time</t>
-  </si>
-  <si>
-    <t>Service Credits</t>
-  </si>
-  <si>
-    <t>Spare Parts Availability</t>
-  </si>
-  <si>
-    <t>Support SLA</t>
-  </si>
-  <si>
-    <t>Warranty Duration</t>
-  </si>
-  <si>
     <t>Unit Price Tier 1</t>
   </si>
   <si>
+    <t>lowest pricing (most optimal)</t>
+  </si>
+  <si>
     <t>Unit Price Tier 2</t>
   </si>
   <si>
+    <t>Mid-level pricing</t>
+  </si>
+  <si>
     <t>Unit Price Tier 3</t>
   </si>
   <si>
+    <t>High-level pricing</t>
+  </si>
+  <si>
     <t>Volume Discount</t>
   </si>
   <si>
+    <t>Range %</t>
+  </si>
+  <si>
     <t>TCO Stability</t>
   </si>
   <si>
-    <t>24 hours</t>
-  </si>
-  <si>
-    <t>3 days</t>
-  </si>
-  <si>
-    <t>7 days</t>
-  </si>
-  <si>
-    <t>Hardware</t>
-  </si>
-  <si>
-    <t>Software</t>
-  </si>
-  <si>
-    <t>Services</t>
-  </si>
-  <si>
-    <t>Field Service</t>
-  </si>
-  <si>
-    <t>Remote Support</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>1 year</t>
-  </si>
-  <si>
-    <t>3 years</t>
-  </si>
-  <si>
-    <t>3-5 years</t>
-  </si>
-  <si>
-    <t>5-7 years</t>
-  </si>
-  <si>
-    <t>7+ years</t>
-  </si>
-  <si>
-    <t>Parent Co</t>
-  </si>
-  <si>
-    <t>Bank Guarantee</t>
-  </si>
-  <si>
-    <t>UK</t>
-  </si>
-  <si>
-    <t>EU</t>
-  </si>
-  <si>
-    <t>Offshore</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Public</t>
-  </si>
-  <si>
-    <t>Private</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>1-2 years</t>
-  </si>
-  <si>
-    <t>&gt;2 years</t>
-  </si>
-  <si>
-    <t>Annual</t>
-  </si>
-  <si>
-    <t>Bi-Annual</t>
-  </si>
-  <si>
-    <t>5-year</t>
-  </si>
-  <si>
-    <t>Ad hoc</t>
-  </si>
-  <si>
-    <t>Included</t>
-  </si>
-  <si>
-    <t>Excluded</t>
-  </si>
-  <si>
-    <t>1 week</t>
-  </si>
-  <si>
-    <t>2 weeks</t>
-  </si>
-  <si>
-    <t>4+ weeks</t>
-  </si>
-  <si>
-    <t>95%</t>
-  </si>
-  <si>
-    <t>98%</t>
-  </si>
-  <si>
-    <t>99.50%</t>
-  </si>
-  <si>
-    <t>Allowed</t>
-  </si>
-  <si>
-    <t>Not Allowed</t>
-  </si>
-  <si>
-    <t>1%</t>
-  </si>
-  <si>
-    <t>2%</t>
-  </si>
-  <si>
-    <t>3%</t>
-  </si>
-  <si>
-    <t>5%</t>
-  </si>
-  <si>
-    <t>10%</t>
-  </si>
-  <si>
-    <t>15%</t>
-  </si>
-  <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>Tiered</t>
-  </si>
-  <si>
-    <t>Flat</t>
-  </si>
-  <si>
-    <t>Global</t>
-  </si>
-  <si>
-    <t>Local Only</t>
-  </si>
-  <si>
-    <t>EU + UK</t>
-  </si>
-  <si>
-    <t>£500k</t>
-  </si>
-  <si>
-    <t>£1M</t>
-  </si>
-  <si>
-    <t>£5M</t>
-  </si>
-  <si>
-    <t>£10M</t>
-  </si>
-  <si>
-    <t>1x contract</t>
-  </si>
-  <si>
-    <t>2x contract</t>
-  </si>
-  <si>
-    <t>Unlimited</t>
-  </si>
-  <si>
-    <t>Internal QA</t>
-  </si>
-  <si>
-    <t>3rd Party Certifier</t>
-  </si>
-  <si>
-    <t>Not Required</t>
-  </si>
-  <si>
-    <t>30 days</t>
-  </si>
-  <si>
-    <t>60 days</t>
-  </si>
-  <si>
-    <t>90 days</t>
-  </si>
-  <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>24 hrs</t>
-  </si>
-  <si>
-    <t>48 hrs</t>
-  </si>
-  <si>
-    <t>72 hrs</t>
-  </si>
-  <si>
-    <t>4 hrs</t>
-  </si>
-  <si>
-    <t>8 hrs</t>
-  </si>
-  <si>
-    <t>Next Day</t>
-  </si>
-  <si>
-    <t>8x5</t>
-  </si>
-  <si>
-    <t>24x5</t>
-  </si>
-  <si>
-    <t>24x7</t>
-  </si>
-  <si>
-    <t>5 years</t>
+    <t>Categorical</t>
+  </si>
+  <si>
+    <t>Total Cost of Ownership (TCO)</t>
   </si>
   <si>
     <t>Inverse Min-Max</t>
   </si>
   <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>10 - ((Supplier TCO - Min TCO) / (Max TCO - Min TCO)) × 10</t>
+  </si>
+  <si>
+    <t>Lower TCO receives a higher score. Auto-scales based on best and worst suppliers.</t>
+  </si>
+  <si>
+    <t>—</t>
+  </si>
+  <si>
+    <t>10 - (Volatility Index × TCO Affected (%) × Adjustment Factor)(e.g. 10 - (3 × 0.6 × 2))</t>
+  </si>
+  <si>
+    <t>Assesses how sensitive TCO is to changes in volume, price escalators, etc.</t>
+  </si>
+  <si>
+    <t>TCO Volatility Index</t>
+  </si>
+  <si>
     <t>Range</t>
   </si>
   <si>
-    <t>Categorical</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
     <t>%</t>
-  </si>
-  <si>
-    <t>Policy Agent</t>
-  </si>
-  <si>
-    <t>Supplier Ranking Agent</t>
-  </si>
-  <si>
-    <t>lowest pricing (most optimal)</t>
-  </si>
-  <si>
-    <t>Mid-level pricing</t>
-  </si>
-  <si>
-    <t>High-level pricing</t>
-  </si>
-  <si>
-    <t>Range %</t>
-  </si>
-  <si>
-    <t>Total Cost of Ownership (TCO)</t>
-  </si>
-  <si>
-    <t>10 - ((Supplier TCO - Min TCO) / (Max TCO - Min TCO)) × 10</t>
-  </si>
-  <si>
-    <t>Lower TCO receives a higher score. Auto-scales based on best and worst suppliers.</t>
-  </si>
-  <si>
-    <t>—</t>
-  </si>
-  <si>
-    <t>Assesses how sensitive TCO is to changes in volume, price escalators, etc.</t>
-  </si>
-  <si>
-    <t>TCO Volatility Index</t>
   </si>
   <si>
     <t>Score = IF(Volatility % ≤ 20%, 8–10, else lower)</t>
@@ -595,12 +617,6 @@
   </si>
   <si>
     <t>Reflects confidence in the demand forecast supporting the TCO estimate.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit </t>
-  </si>
-  <si>
-    <t>10 - (Volatility Index × TCO Affected (%) × Adjustment Factor)(e.g. 10 - (3 × 0.6 × 2))</t>
   </si>
 </sst>
 </file>
@@ -982,16 +998,19 @@
   <dimension ref="A1:O116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" customWidth="1"/>
-    <col min="4" max="4" width="15.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.453125" customWidth="1"/>
-    <col min="9" max="9" width="19.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1008,34 +1027,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -1043,16 +1062,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G2">
         <v>5</v>
@@ -1070,7 +1089,7 @@
         <v>20</v>
       </c>
       <c r="N2" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1078,16 +1097,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>5</v>
@@ -1105,7 +1124,7 @@
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -1113,16 +1132,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G4">
         <v>5</v>
@@ -1140,7 +1159,7 @@
         <v>20</v>
       </c>
       <c r="N4" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -1148,16 +1167,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G5">
         <v>5</v>
@@ -1175,7 +1194,7 @@
         <v>20</v>
       </c>
       <c r="N5" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -1183,16 +1202,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G6">
         <v>5</v>
@@ -1210,7 +1229,7 @@
         <v>20</v>
       </c>
       <c r="N6" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -1218,16 +1237,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G7">
         <v>5</v>
@@ -1245,7 +1264,7 @@
         <v>20</v>
       </c>
       <c r="N7" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -1253,16 +1272,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G8">
         <v>5</v>
@@ -1280,7 +1299,7 @@
         <v>20</v>
       </c>
       <c r="N8" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1288,16 +1307,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G9">
         <v>5</v>
@@ -1315,7 +1334,7 @@
         <v>20</v>
       </c>
       <c r="N9" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1323,16 +1342,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="D10" t="s">
-        <v>75</v>
-      </c>
       <c r="F10" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="G10">
         <v>5</v>
@@ -1350,7 +1369,7 @@
         <v>20</v>
       </c>
       <c r="N10" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1358,16 +1377,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G11">
         <v>4</v>
@@ -1385,7 +1404,7 @@
         <v>24</v>
       </c>
       <c r="N11" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1393,16 +1412,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G12">
         <v>7</v>
@@ -1420,7 +1439,7 @@
         <v>42</v>
       </c>
       <c r="N12" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1428,16 +1447,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G13">
         <v>8</v>
@@ -1455,7 +1474,7 @@
         <v>48</v>
       </c>
       <c r="N13" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1463,16 +1482,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="F14" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G14">
         <v>9</v>
@@ -1490,7 +1509,7 @@
         <v>54</v>
       </c>
       <c r="N14" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1498,16 +1517,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>80</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G15">
         <v>10</v>
@@ -1525,7 +1544,7 @@
         <v>60</v>
       </c>
       <c r="N15" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1533,16 +1552,16 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>38</v>
       </c>
       <c r="F16" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G16">
         <v>5</v>
@@ -1560,7 +1579,7 @@
         <v>30</v>
       </c>
       <c r="N16" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -1568,16 +1587,16 @@
         <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G17">
         <v>5</v>
@@ -1595,7 +1614,7 @@
         <v>30</v>
       </c>
       <c r="N17" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -1603,16 +1622,16 @@
         <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D18" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G18">
         <v>5</v>
@@ -1630,7 +1649,7 @@
         <v>30</v>
       </c>
       <c r="N18" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1638,16 +1657,16 @@
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="F19" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G19">
         <v>5</v>
@@ -1665,7 +1684,7 @@
         <v>30</v>
       </c>
       <c r="N19" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1673,16 +1692,16 @@
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="F20" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G20">
         <v>5</v>
@@ -1700,7 +1719,7 @@
         <v>30</v>
       </c>
       <c r="N20" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1708,16 +1727,16 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G21">
         <v>5</v>
@@ -1735,7 +1754,7 @@
         <v>30</v>
       </c>
       <c r="N21" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1743,16 +1762,16 @@
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" t="s">
         <v>32</v>
-      </c>
-      <c r="D22" t="s">
-        <v>86</v>
-      </c>
-      <c r="F22" t="s">
-        <v>147</v>
       </c>
       <c r="G22">
         <v>10</v>
@@ -1770,7 +1789,7 @@
         <v>60</v>
       </c>
       <c r="N22" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1778,16 +1797,16 @@
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
         <v>32</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" t="s">
-        <v>147</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1805,7 +1824,7 @@
         <v>0</v>
       </c>
       <c r="N23" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1813,16 +1832,16 @@
         <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="F24" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G24">
         <v>5</v>
@@ -1840,7 +1859,7 @@
         <v>30</v>
       </c>
       <c r="N24" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1848,16 +1867,16 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="F25" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G25">
         <v>5</v>
@@ -1875,7 +1894,7 @@
         <v>30</v>
       </c>
       <c r="N25" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1883,16 +1902,16 @@
         <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="F26" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G26">
         <v>10</v>
@@ -1910,7 +1929,7 @@
         <v>60</v>
       </c>
       <c r="N26" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1918,16 +1937,16 @@
         <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="F27" t="s">
-        <v>147</v>
+        <v>32</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1945,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1953,16 +1972,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F28" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G28">
         <v>5</v>
@@ -1980,7 +1999,7 @@
         <v>15</v>
       </c>
       <c r="N28" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1988,16 +2007,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>91</v>
+        <v>55</v>
       </c>
       <c r="F29" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G29">
         <v>5</v>
@@ -2015,7 +2034,7 @@
         <v>15</v>
       </c>
       <c r="N29" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -2023,16 +2042,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="D30" t="s">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="F30" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G30">
         <v>5</v>
@@ -2050,7 +2069,7 @@
         <v>15</v>
       </c>
       <c r="N30" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -2058,16 +2077,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="F31" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G31">
         <v>5</v>
@@ -2085,7 +2104,7 @@
         <v>15</v>
       </c>
       <c r="N31" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -2093,16 +2112,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D32" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="F32" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G32">
         <v>5</v>
@@ -2120,7 +2139,7 @@
         <v>15</v>
       </c>
       <c r="N32" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -2128,16 +2147,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G33">
         <v>5</v>
@@ -2155,7 +2174,7 @@
         <v>15</v>
       </c>
       <c r="N33" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -2163,16 +2182,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="F34" t="s">
-        <v>148</v>
+        <v>54</v>
       </c>
       <c r="G34">
         <v>5</v>
@@ -2190,7 +2209,7 @@
         <v>15</v>
       </c>
       <c r="N34" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -2198,16 +2217,16 @@
         <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>64</v>
       </c>
       <c r="F35" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G35">
         <v>5</v>
@@ -2225,7 +2244,7 @@
         <v>50</v>
       </c>
       <c r="N35" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -2233,16 +2252,16 @@
         <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G36">
         <v>5</v>
@@ -2260,7 +2279,7 @@
         <v>50</v>
       </c>
       <c r="N36" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -2268,16 +2287,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F37" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G37">
         <v>10</v>
@@ -2295,7 +2314,7 @@
         <v>100</v>
       </c>
       <c r="N37" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -2303,16 +2322,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="F38" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G38">
         <v>7</v>
@@ -2330,7 +2349,7 @@
         <v>70</v>
       </c>
       <c r="N38" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -2338,16 +2357,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="F39" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G39">
         <v>3</v>
@@ -2365,7 +2384,7 @@
         <v>30</v>
       </c>
       <c r="N39" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -2373,16 +2392,16 @@
         <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C40" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D40" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="F40" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G40">
         <v>5</v>
@@ -2400,7 +2419,7 @@
         <v>50</v>
       </c>
       <c r="N40" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -2408,16 +2427,16 @@
         <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C41" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D41" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G41">
         <v>5</v>
@@ -2435,7 +2454,7 @@
         <v>50</v>
       </c>
       <c r="N41" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -2443,16 +2462,16 @@
         <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C42" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="D42" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="F42" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G42">
         <v>5</v>
@@ -2470,7 +2489,7 @@
         <v>50</v>
       </c>
       <c r="N42" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -2478,16 +2497,16 @@
         <v>39</v>
       </c>
       <c r="B43" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>105</v>
+        <v>76</v>
       </c>
       <c r="F43" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G43">
         <v>5</v>
@@ -2505,7 +2524,7 @@
         <v>50</v>
       </c>
       <c r="N43" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -2513,16 +2532,16 @@
         <v>40</v>
       </c>
       <c r="B44" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="F44" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G44">
         <v>5</v>
@@ -2540,7 +2559,7 @@
         <v>50</v>
       </c>
       <c r="N44" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2548,16 +2567,16 @@
         <v>50</v>
       </c>
       <c r="B45" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D45" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="F45" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -2575,7 +2594,7 @@
         <v>12</v>
       </c>
       <c r="N45" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -2583,16 +2602,16 @@
         <v>51</v>
       </c>
       <c r="B46" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D46" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="F46" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G46">
         <v>2</v>
@@ -2610,7 +2629,7 @@
         <v>24</v>
       </c>
       <c r="N46" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2618,16 +2637,16 @@
         <v>52</v>
       </c>
       <c r="B47" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D47" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="F47" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G47">
         <v>3</v>
@@ -2645,7 +2664,7 @@
         <v>36</v>
       </c>
       <c r="N47" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2653,16 +2672,16 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C48" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="F48" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G48">
         <v>0</v>
@@ -2680,7 +2699,7 @@
         <v>0</v>
       </c>
       <c r="N48" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:14">
@@ -2688,16 +2707,16 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F49" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G49">
         <v>5</v>
@@ -2721,7 +2740,7 @@
         <v>10000</v>
       </c>
       <c r="N49" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="50" spans="1:14">
@@ -2729,16 +2748,16 @@
         <v>44</v>
       </c>
       <c r="B50" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D50" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="F50" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G50">
         <v>10</v>
@@ -2762,7 +2781,7 @@
         <v>7644</v>
       </c>
       <c r="N50" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:14">
@@ -2770,16 +2789,16 @@
         <v>45</v>
       </c>
       <c r="B51" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D51" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="F51" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G51">
         <v>10</v>
@@ -2803,7 +2822,7 @@
         <v>7671</v>
       </c>
       <c r="N51" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="52" spans="1:14">
@@ -2811,16 +2830,16 @@
         <v>46</v>
       </c>
       <c r="B52" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="D52" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="F52" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G52">
         <v>10</v>
@@ -2844,7 +2863,7 @@
         <v>6195</v>
       </c>
       <c r="N52" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:14">
@@ -2852,16 +2871,16 @@
         <v>47</v>
       </c>
       <c r="B53" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D53" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="F53" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G53">
         <v>5</v>
@@ -2885,7 +2904,7 @@
         <v>9826</v>
       </c>
       <c r="N53" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:14">
@@ -2893,16 +2912,16 @@
         <v>48</v>
       </c>
       <c r="B54" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C54" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
       <c r="F54" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G54">
         <v>5</v>
@@ -2926,7 +2945,7 @@
         <v>2112</v>
       </c>
       <c r="N54" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="1:14">
@@ -2934,16 +2953,16 @@
         <v>49</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="F55" t="s">
-        <v>149</v>
+        <v>65</v>
       </c>
       <c r="G55">
         <v>5</v>
@@ -2967,7 +2986,7 @@
         <v>8347</v>
       </c>
       <c r="N55" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:14">
@@ -2975,16 +2994,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C56" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D56" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="F56" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G56">
         <v>5</v>
@@ -3002,7 +3021,7 @@
         <v>25</v>
       </c>
       <c r="N56" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="57" spans="1:14">
@@ -3010,16 +3029,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D57" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="F57" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G57">
         <v>5</v>
@@ -3037,7 +3056,7 @@
         <v>25</v>
       </c>
       <c r="N57" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="58" spans="1:14">
@@ -3045,16 +3064,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D58" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F58" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G58">
         <v>5</v>
@@ -3072,7 +3091,7 @@
         <v>25</v>
       </c>
       <c r="N58" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="59" spans="1:14">
@@ -3080,16 +3099,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="D59" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="F59" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G59">
         <v>5</v>
@@ -3107,7 +3126,7 @@
         <v>25</v>
       </c>
       <c r="N59" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="60" spans="1:14">
@@ -3115,16 +3134,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="D60" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F60" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G60">
         <v>5</v>
@@ -3142,7 +3161,7 @@
         <v>25</v>
       </c>
       <c r="N60" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="61" spans="1:14">
@@ -3150,16 +3169,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>18</v>
+        <v>92</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="D61" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="F61" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G61">
         <v>5</v>
@@ -3177,7 +3196,7 @@
         <v>25</v>
       </c>
       <c r="N61" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="62" spans="1:14">
@@ -3185,16 +3204,16 @@
         <v>63</v>
       </c>
       <c r="B62" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="D62" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="F62" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G62">
         <v>5</v>
@@ -3212,7 +3231,7 @@
         <v>40</v>
       </c>
       <c r="N62" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="63" spans="1:14">
@@ -3220,16 +3239,16 @@
         <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C63" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="D63" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="F63" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G63">
         <v>5</v>
@@ -3247,7 +3266,7 @@
         <v>40</v>
       </c>
       <c r="N63" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:14">
@@ -3255,16 +3274,16 @@
         <v>65</v>
       </c>
       <c r="B64" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C64" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="D64" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="F64" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G64">
         <v>5</v>
@@ -3282,7 +3301,7 @@
         <v>40</v>
       </c>
       <c r="N64" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:14">
@@ -3290,16 +3309,16 @@
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="D65" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="F65" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G65">
         <v>5</v>
@@ -3317,7 +3336,7 @@
         <v>40</v>
       </c>
       <c r="N65" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:14">
@@ -3325,16 +3344,16 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="D66" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="F66" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G66">
         <v>5</v>
@@ -3352,7 +3371,7 @@
         <v>40</v>
       </c>
       <c r="N66" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:14">
@@ -3360,16 +3379,16 @@
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C67" t="s">
-        <v>47</v>
+        <v>104</v>
       </c>
       <c r="D67" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="F67" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G67">
         <v>5</v>
@@ -3387,7 +3406,7 @@
         <v>40</v>
       </c>
       <c r="N67" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:14">
@@ -3395,16 +3414,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C68" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="D68" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="F68" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G68">
         <v>6</v>
@@ -3422,7 +3441,7 @@
         <v>48</v>
       </c>
       <c r="N68" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="69" spans="1:14">
@@ -3430,16 +3449,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C69" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="D69" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="F69" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G69">
         <v>8</v>
@@ -3457,7 +3476,7 @@
         <v>64</v>
       </c>
       <c r="N69" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="70" spans="1:14">
@@ -3465,16 +3484,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>19</v>
+        <v>99</v>
       </c>
       <c r="C70" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="D70" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="F70" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G70">
         <v>10</v>
@@ -3492,7 +3511,7 @@
         <v>80</v>
       </c>
       <c r="N70" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="71" spans="1:14">
@@ -3500,16 +3519,16 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="D71" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="F71" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G71">
         <v>5</v>
@@ -3527,7 +3546,7 @@
         <v>25</v>
       </c>
       <c r="N71" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:14">
@@ -3535,16 +3554,16 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C72" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="D72" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="F72" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G72">
         <v>5</v>
@@ -3562,7 +3581,7 @@
         <v>25</v>
       </c>
       <c r="N72" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:14">
@@ -3570,16 +3589,16 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="D73" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="F73" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G73">
         <v>5</v>
@@ -3597,7 +3616,7 @@
         <v>25</v>
       </c>
       <c r="N73" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:14">
@@ -3605,16 +3624,16 @@
         <v>69</v>
       </c>
       <c r="B74" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="D74" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="F74" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G74">
         <v>10</v>
@@ -3632,7 +3651,7 @@
         <v>50</v>
       </c>
       <c r="N74" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:14">
@@ -3640,16 +3659,16 @@
         <v>70</v>
       </c>
       <c r="B75" t="s">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="C75" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="D75" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="F75" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="G75">
         <v>0</v>
@@ -3667,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="N75" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="76" spans="1:14">
@@ -3675,13 +3694,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C76" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="D76" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F76">
         <v>10</v>
@@ -3702,7 +3721,7 @@
         <v>100</v>
       </c>
       <c r="N76" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:14">
@@ -3710,13 +3729,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C77" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="D77" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="F77">
         <v>10</v>
@@ -3737,7 +3756,7 @@
         <v>50</v>
       </c>
       <c r="N77" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:14">
@@ -3745,13 +3764,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C78" t="s">
-        <v>51</v>
+        <v>118</v>
       </c>
       <c r="D78" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="F78">
         <v>10</v>
@@ -3772,7 +3791,7 @@
         <v>20</v>
       </c>
       <c r="N78" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:14">
@@ -3780,13 +3799,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C79" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="D79" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F79">
         <v>10</v>
@@ -3807,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="N79" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:14">
@@ -3815,13 +3834,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C80" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="D80" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="F80">
         <v>10</v>
@@ -3842,7 +3861,7 @@
         <v>10</v>
       </c>
       <c r="N80" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="81" spans="1:14">
@@ -3850,13 +3869,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C81" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="D81" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="F81">
         <v>10</v>
@@ -3877,7 +3896,7 @@
         <v>20</v>
       </c>
       <c r="N81" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:14">
@@ -3885,13 +3904,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="C82" t="s">
-        <v>52</v>
+        <v>122</v>
       </c>
       <c r="D82" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="F82">
         <v>10</v>
@@ -3912,7 +3931,7 @@
         <v>30</v>
       </c>
       <c r="N82" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:14">
@@ -3920,16 +3939,16 @@
         <v>100</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="D83" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="F83" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G83">
         <v>10</v>
@@ -3947,7 +3966,7 @@
         <v>80</v>
       </c>
       <c r="N83" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:14">
@@ -3955,16 +3974,16 @@
         <v>101</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C84" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="D84" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="F84" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -3982,7 +4001,7 @@
         <v>0</v>
       </c>
       <c r="N84" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:14">
@@ -3990,16 +4009,16 @@
         <v>102</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C85" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="D85" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="F85" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G85">
         <v>10</v>
@@ -4017,7 +4036,7 @@
         <v>80</v>
       </c>
       <c r="N85" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:14">
@@ -4025,16 +4044,16 @@
         <v>103</v>
       </c>
       <c r="B86" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C86" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="D86" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="F86" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G86">
         <v>0</v>
@@ -4052,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="N86" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="87" spans="1:14">
@@ -4060,16 +4079,16 @@
         <v>104</v>
       </c>
       <c r="B87" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C87" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="D87" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="F87" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G87">
         <v>10</v>
@@ -4087,7 +4106,7 @@
         <v>80</v>
       </c>
       <c r="N87" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -4095,16 +4114,16 @@
         <v>105</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>124</v>
       </c>
       <c r="C88" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="D88" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="F88" t="s">
-        <v>151</v>
+        <v>102</v>
       </c>
       <c r="G88">
         <v>0</v>
@@ -4122,7 +4141,7 @@
         <v>0</v>
       </c>
       <c r="N88" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="89" spans="1:14">
@@ -4130,16 +4149,16 @@
         <v>93</v>
       </c>
       <c r="B89" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C89" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="D89" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F89" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G89">
         <v>10</v>
@@ -4157,7 +4176,7 @@
         <v>90</v>
       </c>
       <c r="N89" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -4165,16 +4184,16 @@
         <v>94</v>
       </c>
       <c r="B90" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C90" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="D90" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F90" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G90">
         <v>7</v>
@@ -4192,7 +4211,7 @@
         <v>63</v>
       </c>
       <c r="N90" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="91" spans="1:14">
@@ -4200,16 +4219,16 @@
         <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C91" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
       <c r="D91" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F91" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G91">
         <v>5</v>
@@ -4227,7 +4246,7 @@
         <v>45</v>
       </c>
       <c r="N91" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="92" spans="1:14">
@@ -4235,16 +4254,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C92" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="D92" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F92" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G92">
         <v>10</v>
@@ -4262,7 +4281,7 @@
         <v>90</v>
       </c>
       <c r="N92" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="93" spans="1:14">
@@ -4270,16 +4289,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C93" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="D93" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F93" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G93">
         <v>7</v>
@@ -4297,7 +4316,7 @@
         <v>63</v>
       </c>
       <c r="N93" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="94" spans="1:14">
@@ -4305,16 +4324,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C94" t="s">
-        <v>57</v>
+        <v>134</v>
       </c>
       <c r="D94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F94" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G94">
         <v>4</v>
@@ -4332,7 +4351,7 @@
         <v>36</v>
       </c>
       <c r="N94" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="95" spans="1:14">
@@ -4340,16 +4359,16 @@
         <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C95" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="D95" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
       <c r="F95" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G95">
         <v>5</v>
@@ -4373,7 +4392,7 @@
         <v>4365</v>
       </c>
       <c r="N95" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="96" spans="1:14">
@@ -4381,16 +4400,16 @@
         <v>97</v>
       </c>
       <c r="B96" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C96" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="D96" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="F96" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G96">
         <v>10</v>
@@ -4414,7 +4433,7 @@
         <v>10888</v>
       </c>
       <c r="N96" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -4422,16 +4441,16 @@
         <v>98</v>
       </c>
       <c r="B97" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C97" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="D97" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
       <c r="F97" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G97">
         <v>10</v>
@@ -4455,7 +4474,7 @@
         <v>2677</v>
       </c>
       <c r="N97" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -4463,16 +4482,16 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
+        <v>128</v>
       </c>
       <c r="C98" t="s">
-        <v>58</v>
+        <v>138</v>
       </c>
       <c r="D98" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="F98" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -4496,7 +4515,7 @@
         <v>5799</v>
       </c>
       <c r="N98" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -4504,16 +4523,16 @@
         <v>87</v>
       </c>
       <c r="B99" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="D99" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="F99" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G99">
         <v>10</v>
@@ -4531,7 +4550,7 @@
         <v>70</v>
       </c>
       <c r="N99" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -4539,16 +4558,16 @@
         <v>88</v>
       </c>
       <c r="B100" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C100" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="D100" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="F100" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G100">
         <v>7</v>
@@ -4566,7 +4585,7 @@
         <v>49</v>
       </c>
       <c r="N100" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="101" spans="1:14">
@@ -4574,16 +4593,16 @@
         <v>89</v>
       </c>
       <c r="B101" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C101" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
       <c r="D101" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="F101" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G101">
         <v>3</v>
@@ -4601,7 +4620,7 @@
         <v>21</v>
       </c>
       <c r="N101" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:14">
@@ -4609,16 +4628,16 @@
         <v>84</v>
       </c>
       <c r="B102" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C102" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="D102" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="F102" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G102">
         <v>5</v>
@@ -4636,7 +4655,7 @@
         <v>35</v>
       </c>
       <c r="N102" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:14">
@@ -4644,16 +4663,16 @@
         <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C103" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="D103" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="F103" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G103">
         <v>7</v>
@@ -4671,7 +4690,7 @@
         <v>49</v>
       </c>
       <c r="N103" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="104" spans="1:14">
@@ -4679,16 +4698,16 @@
         <v>86</v>
       </c>
       <c r="B104" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C104" t="s">
-        <v>60</v>
+        <v>142</v>
       </c>
       <c r="D104" t="s">
+        <v>145</v>
+      </c>
+      <c r="F104" t="s">
         <v>141</v>
-      </c>
-      <c r="F104" t="s">
-        <v>153</v>
       </c>
       <c r="G104">
         <v>10</v>
@@ -4706,7 +4725,7 @@
         <v>70</v>
       </c>
       <c r="N104" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="105" spans="1:14">
@@ -4714,16 +4733,16 @@
         <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C105" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="D105" t="s">
-        <v>76</v>
+        <v>31</v>
       </c>
       <c r="F105" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G105">
         <v>5</v>
@@ -4741,7 +4760,7 @@
         <v>35</v>
       </c>
       <c r="N105" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="1:14">
@@ -4749,16 +4768,16 @@
         <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C106" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="D106" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="F106" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G106">
         <v>8</v>
@@ -4776,7 +4795,7 @@
         <v>56</v>
       </c>
       <c r="N106" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="107" spans="1:14">
@@ -4784,16 +4803,16 @@
         <v>83</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>139</v>
       </c>
       <c r="C107" t="s">
-        <v>61</v>
+        <v>146</v>
       </c>
       <c r="D107" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="F107" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="G107">
         <v>10</v>
@@ -4811,7 +4830,7 @@
         <v>70</v>
       </c>
       <c r="N107" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="108" spans="1:14">
@@ -4819,13 +4838,13 @@
         <v>84</v>
       </c>
       <c r="B108" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C108" t="s">
-        <v>62</v>
+        <v>149</v>
       </c>
       <c r="D108" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="F108">
         <v>10</v>
@@ -4837,7 +4856,7 @@
         <v>100</v>
       </c>
       <c r="N108" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="109" spans="1:14">
@@ -4845,13 +4864,13 @@
         <v>85</v>
       </c>
       <c r="B109" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C109" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="D109" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="F109">
         <v>8</v>
@@ -4863,7 +4882,7 @@
         <v>56</v>
       </c>
       <c r="N109" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="110" spans="1:14">
@@ -4871,13 +4890,13 @@
         <v>86</v>
       </c>
       <c r="B110" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C110" t="s">
-        <v>64</v>
+        <v>153</v>
       </c>
       <c r="D110" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="F110">
         <v>6</v>
@@ -4889,7 +4908,7 @@
         <v>24</v>
       </c>
       <c r="N110" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="111" spans="1:14">
@@ -4897,13 +4916,13 @@
         <v>87</v>
       </c>
       <c r="B111" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C111" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
       <c r="D111" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F111">
         <v>8</v>
@@ -4915,7 +4934,7 @@
         <v>48</v>
       </c>
       <c r="N111" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
     </row>
     <row r="112" spans="1:14">
@@ -4923,123 +4942,135 @@
         <v>88</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C112" t="s">
-        <v>66</v>
+        <v>157</v>
       </c>
       <c r="D112" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="G112">
         <v>3</v>
       </c>
       <c r="N112" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="113" spans="2:15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="113" spans="1:15">
+      <c r="A113">
+        <v>89</v>
+      </c>
       <c r="B113" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C113" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D113" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="E113" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="F113">
         <v>9</v>
       </c>
       <c r="G113" t="s">
+        <v>162</v>
+      </c>
+      <c r="N113" t="s">
+        <v>81</v>
+      </c>
+      <c r="O113" t="s">
         <v>163</v>
       </c>
-      <c r="N113" t="s">
+    </row>
+    <row r="114" spans="1:15">
+      <c r="A114">
+        <v>90</v>
+      </c>
+      <c r="B114" t="s">
+        <v>148</v>
+      </c>
+      <c r="C114" t="s">
         <v>157</v>
       </c>
-      <c r="O113" t="s">
+      <c r="D114" t="s">
+        <v>158</v>
+      </c>
+      <c r="E114" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="114" spans="2:15">
-      <c r="B114" t="s">
-        <v>25</v>
-      </c>
-      <c r="C114" t="s">
-        <v>66</v>
-      </c>
-      <c r="D114" t="s">
-        <v>145</v>
-      </c>
-      <c r="E114" t="s">
-        <v>165</v>
       </c>
       <c r="F114">
         <v>6</v>
       </c>
       <c r="G114" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="N114" t="s">
-        <v>157</v>
+        <v>81</v>
       </c>
       <c r="O114" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="115" spans="2:15">
+    <row r="115" spans="1:15">
+      <c r="A115">
+        <v>91</v>
+      </c>
       <c r="B115" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C115" t="s">
         <v>167</v>
       </c>
       <c r="D115" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E115" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="F115">
         <v>4</v>
       </c>
       <c r="G115" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="N115" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="O115" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="116" spans="2:15">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116">
+        <v>92</v>
+      </c>
       <c r="B116" t="s">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="C116" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D116" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="E116" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F116">
         <v>5</v>
       </c>
       <c r="G116" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="N116" t="s">
-        <v>156</v>
+        <v>18</v>
       </c>
       <c r="O116" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -5258,45 +5289,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3364095-52D0-423F-A96C-8D43873368DC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="7374e2ad-90c5-41fd-a998-011aaae8d148"/>
-    <ds:schemaRef ds:uri="66e99abc-29ec-44c5-b05d-8ae112ecdef3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3364095-52D0-423F-A96C-8D43873368DC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E4DD928-E199-452E-8B48-9288407D4847}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E4DD928-E199-452E-8B48-9288407D4847}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE73188F-7D73-45AB-9055-8593A3E689CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="66e99abc-29ec-44c5-b05d-8ae112ecdef3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7374e2ad-90c5-41fd-a998-011aaae8d148"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FE73188F-7D73-45AB-9055-8593A3E689CF}"/>
 </file>
</xml_diff>